<commit_message>
Custom file excel modified
</commit_message>
<xml_diff>
--- a/public/Custom_file_users.xlsx
+++ b/public/Custom_file_users.xlsx
@@ -79,9 +79,6 @@
     <t>user_email6@ext.com</t>
   </si>
   <si>
-    <t>user_email7ext.com</t>
-  </si>
-  <si>
     <t>user_email8@ext.com</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>pass123456800</t>
+  </si>
+  <si>
+    <t>user_email7@ext.com</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -516,7 +516,7 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -527,7 +527,7 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -538,7 +538,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -549,7 +549,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -560,7 +560,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -571,7 +571,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -579,10 +579,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -590,10 +590,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -601,10 +601,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -613,10 +613,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -624,10 +624,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -635,10 +635,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -655,8 +655,9 @@
     <hyperlink ref="B10" r:id="rId10"/>
     <hyperlink ref="B11" r:id="rId11"/>
     <hyperlink ref="B12" r:id="rId12"/>
+    <hyperlink ref="B8" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>